<commit_message>
Thắng commit số công Code
</commit_message>
<xml_diff>
--- a/2015/201510/20_MANAGEMENT/SOF.QP.03.F05_TaskList - TAX.xlsx
+++ b/2015/201510/20_MANAGEMENT/SOF.QP.03.F05_TaskList - TAX.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2160"/>
@@ -9,9 +9,9 @@
   <sheets>
     <sheet name="Tasks" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="144525"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -344,6 +344,28 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -364,28 +386,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -757,18 +757,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -782,12 +782,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
@@ -796,20 +796,20 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
@@ -843,212 +843,234 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6">
+        <v>40</v>
+      </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="15">
-      <c r="A7" s="20"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6">
+        <v>40</v>
+      </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="15">
-      <c r="A8" s="20"/>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6">
+        <v>16</v>
+      </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" ht="15">
-      <c r="A9" s="20"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6">
+        <v>24</v>
+      </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6">
+        <v>24</v>
+      </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="15">
-      <c r="A12" s="20"/>
-      <c r="B12" s="18" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" ht="15">
-      <c r="A13" s="20"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="15">
-      <c r="A14" s="20"/>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="15">
-      <c r="A15" s="20"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" ht="15">
-      <c r="A16" s="20"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="22"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="15">
-      <c r="A17" s="20"/>
-      <c r="B17" s="18" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="15">
-      <c r="A18" s="20"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="15">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6">
+        <v>16</v>
+      </c>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="15">
-      <c r="A21" s="20"/>
-      <c r="B21" s="18" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="22"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6">
+        <v>16</v>
+      </c>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="30">
-      <c r="A22" s="20"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
+      <c r="E22" s="6">
+        <v>24</v>
+      </c>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="15">
-      <c r="A23" s="20"/>
-      <c r="B23" s="18" t="s">
+      <c r="A23" s="12"/>
+      <c r="B23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6">
+        <v>24</v>
+      </c>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" ht="15">
-      <c r="A24" s="20"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
+      <c r="E24" s="6">
+        <v>24</v>
+      </c>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10">
+        <v>80</v>
+      </c>
+      <c r="F25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Huyền cập nhật số công thực hiện
</commit_message>
<xml_diff>
--- a/2015/201510/20_MANAGEMENT/SOF.QP.03.F05_TaskList - TAX.xlsx
+++ b/2015/201510/20_MANAGEMENT/SOF.QP.03.F05_TaskList - TAX.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THUC TAP\SVN_Test\20_MANAGEMENT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2160"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -757,7 +762,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -767,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -915,7 +920,9 @@
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6">
+        <v>5</v>
+      </c>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="15">
@@ -925,7 +932,9 @@
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="6">
+        <v>12</v>
+      </c>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" ht="15">
@@ -935,7 +944,9 @@
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6">
+        <v>24</v>
+      </c>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="15">
@@ -945,7 +956,9 @@
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="6">
+        <v>12</v>
+      </c>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -955,7 +968,9 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
+      <c r="E15" s="6">
+        <v>24</v>
+      </c>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" ht="15">
@@ -965,7 +980,9 @@
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6">
+        <v>20</v>
+      </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="15">
@@ -975,7 +992,9 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6">
+        <v>80</v>
+      </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="15">
@@ -985,7 +1004,9 @@
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6">
+        <v>24</v>
+      </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="15">
@@ -995,7 +1016,9 @@
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6">
+        <v>24</v>
+      </c>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1">

</xml_diff>